<commit_message>
updated datasheet finished, 2020.12.14 IC-C1 transects 1 and 2
</commit_message>
<xml_diff>
--- a/fishSurveys/data/fishSurveyData.xlsx
+++ b/fishSurveys/data/fishSurveyData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="143">
   <si>
     <t>date</t>
   </si>
@@ -322,6 +322,129 @@
   </si>
   <si>
     <t>Stegastes adustus</t>
+  </si>
+  <si>
+    <t>GOPR0195.MP4008.png</t>
+  </si>
+  <si>
+    <t>Thalassoma</t>
+  </si>
+  <si>
+    <t>GOPR0195.MP4009.png</t>
+  </si>
+  <si>
+    <t>Haelumon carbonarium</t>
+  </si>
+  <si>
+    <t>GOPR0195.MP4010.png</t>
+  </si>
+  <si>
+    <t>GOPR0195.MP4011.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stegastes </t>
+  </si>
+  <si>
+    <t>Spanish Hogfish</t>
+  </si>
+  <si>
+    <t>Bodianus</t>
+  </si>
+  <si>
+    <t>rufus</t>
+  </si>
+  <si>
+    <t>Bodianus rufus</t>
+  </si>
+  <si>
+    <t>Foureye Butterflyfish</t>
+  </si>
+  <si>
+    <t>capistratus</t>
+  </si>
+  <si>
+    <t>Chaetodon capistratus</t>
+  </si>
+  <si>
+    <t>Painted Wrasse</t>
+  </si>
+  <si>
+    <t>Halichoeres</t>
+  </si>
+  <si>
+    <t>caudalis</t>
+  </si>
+  <si>
+    <t>Halichoeres caudalis</t>
+  </si>
+  <si>
+    <t>GOPR0195.MP4012.png</t>
+  </si>
+  <si>
+    <t>Foureye butterflyfish</t>
+  </si>
+  <si>
+    <t>GOPR0195.MP4013.png</t>
+  </si>
+  <si>
+    <t>GOPR0195.MP4014.png</t>
+  </si>
+  <si>
+    <t>GOPR0195.MP4015.png</t>
+  </si>
+  <si>
+    <t>GOPR0195.MP4016.png</t>
+  </si>
+  <si>
+    <t>GOPR0195.MP4017.png</t>
+  </si>
+  <si>
+    <t>Segastes partitus</t>
+  </si>
+  <si>
+    <t>GOPR0195.MP4018.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slippery Dick </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Halichoeres </t>
+  </si>
+  <si>
+    <t>bivittatus</t>
+  </si>
+  <si>
+    <t>Halichoeres bivittatus</t>
+  </si>
+  <si>
+    <t>GOPR0195.MP4019.png</t>
+  </si>
+  <si>
+    <t>GOPR0195.MP4020.png</t>
+  </si>
+  <si>
+    <t>Haemulon pulmierii</t>
+  </si>
+  <si>
+    <t>Parrotfish</t>
+  </si>
+  <si>
+    <t>UNK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">both individuals unidentifiable </t>
+  </si>
+  <si>
+    <t>GOPR0195.MP4021.png</t>
+  </si>
+  <si>
+    <t>GOPR0195.MP4022.png</t>
+  </si>
+  <si>
+    <t>individual unidentifiable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">individual unidentifiable </t>
   </si>
 </sst>
 </file>
@@ -667,11 +790,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W45"/>
+  <dimension ref="A1:W83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J45" sqref="J45"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M83" sqref="M83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2139,6 +2262,15 @@
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B43" t="s">
+        <v>18</v>
+      </c>
+      <c r="C43">
+        <v>2</v>
+      </c>
       <c r="D43">
         <v>3</v>
       </c>
@@ -2162,6 +2294,21 @@
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B44" t="s">
+        <v>18</v>
+      </c>
+      <c r="C44">
+        <v>2</v>
+      </c>
+      <c r="D44">
+        <v>3</v>
+      </c>
+      <c r="E44" t="s">
+        <v>98</v>
+      </c>
       <c r="F44" t="s">
         <v>51</v>
       </c>
@@ -2179,6 +2326,21 @@
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B45" t="s">
+        <v>18</v>
+      </c>
+      <c r="C45">
+        <v>2</v>
+      </c>
+      <c r="D45">
+        <v>3</v>
+      </c>
+      <c r="E45" t="s">
+        <v>98</v>
+      </c>
       <c r="F45" t="s">
         <v>99</v>
       </c>
@@ -2193,6 +2355,1270 @@
       </c>
       <c r="J45">
         <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B46" t="s">
+        <v>18</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
+      </c>
+      <c r="D46">
+        <v>3</v>
+      </c>
+      <c r="E46" t="s">
+        <v>98</v>
+      </c>
+      <c r="F46" t="s">
+        <v>87</v>
+      </c>
+      <c r="G46" t="s">
+        <v>88</v>
+      </c>
+      <c r="H46" t="s">
+        <v>89</v>
+      </c>
+      <c r="I46" t="s">
+        <v>90</v>
+      </c>
+      <c r="J46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B47" t="s">
+        <v>18</v>
+      </c>
+      <c r="C47">
+        <v>2</v>
+      </c>
+      <c r="D47">
+        <v>4</v>
+      </c>
+      <c r="E47" t="s">
+        <v>102</v>
+      </c>
+      <c r="F47" t="s">
+        <v>87</v>
+      </c>
+      <c r="G47" t="s">
+        <v>88</v>
+      </c>
+      <c r="H47" t="s">
+        <v>89</v>
+      </c>
+      <c r="I47" t="s">
+        <v>90</v>
+      </c>
+      <c r="J47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B48" t="s">
+        <v>18</v>
+      </c>
+      <c r="C48">
+        <v>2</v>
+      </c>
+      <c r="D48">
+        <v>4</v>
+      </c>
+      <c r="E48" t="s">
+        <v>102</v>
+      </c>
+      <c r="F48" t="s">
+        <v>25</v>
+      </c>
+      <c r="G48" t="s">
+        <v>47</v>
+      </c>
+      <c r="H48" t="s">
+        <v>26</v>
+      </c>
+      <c r="I48" t="s">
+        <v>27</v>
+      </c>
+      <c r="J48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B49" t="s">
+        <v>18</v>
+      </c>
+      <c r="C49">
+        <v>2</v>
+      </c>
+      <c r="D49">
+        <v>4</v>
+      </c>
+      <c r="E49" t="s">
+        <v>102</v>
+      </c>
+      <c r="F49" t="s">
+        <v>39</v>
+      </c>
+      <c r="G49" t="s">
+        <v>103</v>
+      </c>
+      <c r="H49" t="s">
+        <v>41</v>
+      </c>
+      <c r="I49" t="s">
+        <v>40</v>
+      </c>
+      <c r="J49">
+        <v>1</v>
+      </c>
+      <c r="L49" t="s">
+        <v>73</v>
+      </c>
+      <c r="M49" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B50" t="s">
+        <v>18</v>
+      </c>
+      <c r="C50">
+        <v>2</v>
+      </c>
+      <c r="D50">
+        <v>5</v>
+      </c>
+      <c r="E50" t="s">
+        <v>104</v>
+      </c>
+      <c r="F50" t="s">
+        <v>51</v>
+      </c>
+      <c r="G50" t="s">
+        <v>21</v>
+      </c>
+      <c r="H50" t="s">
+        <v>52</v>
+      </c>
+      <c r="I50" t="s">
+        <v>105</v>
+      </c>
+      <c r="J50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B51" t="s">
+        <v>18</v>
+      </c>
+      <c r="C51">
+        <v>2</v>
+      </c>
+      <c r="D51">
+        <v>6</v>
+      </c>
+      <c r="E51" t="s">
+        <v>106</v>
+      </c>
+      <c r="F51" t="s">
+        <v>87</v>
+      </c>
+      <c r="G51" t="s">
+        <v>88</v>
+      </c>
+      <c r="H51" t="s">
+        <v>89</v>
+      </c>
+      <c r="I51" t="s">
+        <v>90</v>
+      </c>
+      <c r="J51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B52" t="s">
+        <v>18</v>
+      </c>
+      <c r="C52">
+        <v>2</v>
+      </c>
+      <c r="D52">
+        <v>6</v>
+      </c>
+      <c r="E52" t="s">
+        <v>106</v>
+      </c>
+      <c r="F52" t="s">
+        <v>39</v>
+      </c>
+      <c r="G52" t="s">
+        <v>103</v>
+      </c>
+      <c r="H52" t="s">
+        <v>41</v>
+      </c>
+      <c r="I52" t="s">
+        <v>40</v>
+      </c>
+      <c r="J52">
+        <v>2</v>
+      </c>
+      <c r="L52" t="s">
+        <v>73</v>
+      </c>
+      <c r="M52" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B53" t="s">
+        <v>18</v>
+      </c>
+      <c r="C53">
+        <v>2</v>
+      </c>
+      <c r="D53">
+        <v>7</v>
+      </c>
+      <c r="E53" t="s">
+        <v>107</v>
+      </c>
+      <c r="F53" t="s">
+        <v>87</v>
+      </c>
+      <c r="G53" t="s">
+        <v>108</v>
+      </c>
+      <c r="H53" t="s">
+        <v>89</v>
+      </c>
+      <c r="I53" t="s">
+        <v>90</v>
+      </c>
+      <c r="J53">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B54" t="s">
+        <v>18</v>
+      </c>
+      <c r="C54">
+        <v>2</v>
+      </c>
+      <c r="D54">
+        <v>7</v>
+      </c>
+      <c r="E54" t="s">
+        <v>107</v>
+      </c>
+      <c r="F54" t="s">
+        <v>109</v>
+      </c>
+      <c r="G54" t="s">
+        <v>110</v>
+      </c>
+      <c r="H54" t="s">
+        <v>111</v>
+      </c>
+      <c r="I54" t="s">
+        <v>112</v>
+      </c>
+      <c r="J54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B55" t="s">
+        <v>18</v>
+      </c>
+      <c r="C55">
+        <v>2</v>
+      </c>
+      <c r="D55">
+        <v>7</v>
+      </c>
+      <c r="E55" t="s">
+        <v>107</v>
+      </c>
+      <c r="F55" t="s">
+        <v>39</v>
+      </c>
+      <c r="G55" t="s">
+        <v>103</v>
+      </c>
+      <c r="H55" t="s">
+        <v>41</v>
+      </c>
+      <c r="I55" t="s">
+        <v>40</v>
+      </c>
+      <c r="J55">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B56" t="s">
+        <v>18</v>
+      </c>
+      <c r="C56">
+        <v>2</v>
+      </c>
+      <c r="D56">
+        <v>7</v>
+      </c>
+      <c r="E56" t="s">
+        <v>107</v>
+      </c>
+      <c r="F56" t="s">
+        <v>113</v>
+      </c>
+      <c r="G56" t="s">
+        <v>59</v>
+      </c>
+      <c r="H56" t="s">
+        <v>114</v>
+      </c>
+      <c r="I56" t="s">
+        <v>115</v>
+      </c>
+      <c r="J56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B57" t="s">
+        <v>18</v>
+      </c>
+      <c r="C57">
+        <v>2</v>
+      </c>
+      <c r="D57">
+        <v>7</v>
+      </c>
+      <c r="E57" t="s">
+        <v>107</v>
+      </c>
+      <c r="F57" t="s">
+        <v>116</v>
+      </c>
+      <c r="G57" t="s">
+        <v>117</v>
+      </c>
+      <c r="H57" t="s">
+        <v>118</v>
+      </c>
+      <c r="I57" t="s">
+        <v>119</v>
+      </c>
+      <c r="J57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B58" t="s">
+        <v>18</v>
+      </c>
+      <c r="C58">
+        <v>2</v>
+      </c>
+      <c r="D58">
+        <v>8</v>
+      </c>
+      <c r="E58" t="s">
+        <v>120</v>
+      </c>
+      <c r="F58" t="s">
+        <v>116</v>
+      </c>
+      <c r="G58" t="s">
+        <v>117</v>
+      </c>
+      <c r="H58" t="s">
+        <v>118</v>
+      </c>
+      <c r="I58" t="s">
+        <v>119</v>
+      </c>
+      <c r="J58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B59" t="s">
+        <v>18</v>
+      </c>
+      <c r="C59">
+        <v>2</v>
+      </c>
+      <c r="D59">
+        <v>8</v>
+      </c>
+      <c r="E59" t="s">
+        <v>120</v>
+      </c>
+      <c r="F59" t="s">
+        <v>121</v>
+      </c>
+      <c r="G59" t="s">
+        <v>33</v>
+      </c>
+      <c r="H59" t="s">
+        <v>114</v>
+      </c>
+      <c r="I59" t="s">
+        <v>115</v>
+      </c>
+      <c r="J59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B60" t="s">
+        <v>18</v>
+      </c>
+      <c r="C60">
+        <v>2</v>
+      </c>
+      <c r="D60">
+        <v>8</v>
+      </c>
+      <c r="E60" t="s">
+        <v>120</v>
+      </c>
+      <c r="F60" t="s">
+        <v>87</v>
+      </c>
+      <c r="G60" t="s">
+        <v>88</v>
+      </c>
+      <c r="H60" t="s">
+        <v>89</v>
+      </c>
+      <c r="I60" t="s">
+        <v>90</v>
+      </c>
+      <c r="J60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B61" t="s">
+        <v>18</v>
+      </c>
+      <c r="C61">
+        <v>2</v>
+      </c>
+      <c r="D61">
+        <v>8</v>
+      </c>
+      <c r="E61" t="s">
+        <v>120</v>
+      </c>
+      <c r="F61" t="s">
+        <v>39</v>
+      </c>
+      <c r="G61" t="s">
+        <v>103</v>
+      </c>
+      <c r="H61" t="s">
+        <v>41</v>
+      </c>
+      <c r="I61" t="s">
+        <v>40</v>
+      </c>
+      <c r="J61">
+        <v>2</v>
+      </c>
+      <c r="L61" t="s">
+        <v>73</v>
+      </c>
+      <c r="M61" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A62" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B62" t="s">
+        <v>18</v>
+      </c>
+      <c r="C62">
+        <v>2</v>
+      </c>
+      <c r="D62">
+        <v>9</v>
+      </c>
+      <c r="E62" t="s">
+        <v>122</v>
+      </c>
+      <c r="F62" t="s">
+        <v>39</v>
+      </c>
+      <c r="G62" t="s">
+        <v>103</v>
+      </c>
+      <c r="H62" t="s">
+        <v>41</v>
+      </c>
+      <c r="I62" t="s">
+        <v>40</v>
+      </c>
+      <c r="J62">
+        <v>2</v>
+      </c>
+      <c r="L62" t="s">
+        <v>73</v>
+      </c>
+      <c r="M62" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A63" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B63" t="s">
+        <v>18</v>
+      </c>
+      <c r="C63">
+        <v>2</v>
+      </c>
+      <c r="D63">
+        <v>9</v>
+      </c>
+      <c r="E63" t="s">
+        <v>122</v>
+      </c>
+      <c r="F63" t="s">
+        <v>116</v>
+      </c>
+      <c r="G63" t="s">
+        <v>117</v>
+      </c>
+      <c r="H63" t="s">
+        <v>118</v>
+      </c>
+      <c r="I63" t="s">
+        <v>119</v>
+      </c>
+      <c r="J63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B64" t="s">
+        <v>18</v>
+      </c>
+      <c r="C64">
+        <v>2</v>
+      </c>
+      <c r="D64">
+        <v>10</v>
+      </c>
+      <c r="E64" t="s">
+        <v>123</v>
+      </c>
+      <c r="F64" t="s">
+        <v>69</v>
+      </c>
+      <c r="G64" t="s">
+        <v>69</v>
+      </c>
+      <c r="H64" t="s">
+        <v>69</v>
+      </c>
+      <c r="I64" t="s">
+        <v>69</v>
+      </c>
+      <c r="J64" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A65" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B65" t="s">
+        <v>18</v>
+      </c>
+      <c r="C65">
+        <v>2</v>
+      </c>
+      <c r="D65">
+        <v>11</v>
+      </c>
+      <c r="E65" t="s">
+        <v>124</v>
+      </c>
+      <c r="F65" t="s">
+        <v>87</v>
+      </c>
+      <c r="G65" t="s">
+        <v>88</v>
+      </c>
+      <c r="H65" t="s">
+        <v>89</v>
+      </c>
+      <c r="I65" t="s">
+        <v>90</v>
+      </c>
+      <c r="J65">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A66" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B66" t="s">
+        <v>18</v>
+      </c>
+      <c r="C66">
+        <v>2</v>
+      </c>
+      <c r="D66">
+        <v>11</v>
+      </c>
+      <c r="E66" t="s">
+        <v>124</v>
+      </c>
+      <c r="F66" t="s">
+        <v>116</v>
+      </c>
+      <c r="G66" t="s">
+        <v>117</v>
+      </c>
+      <c r="H66" t="s">
+        <v>118</v>
+      </c>
+      <c r="I66" t="s">
+        <v>119</v>
+      </c>
+      <c r="J66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A67" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B67" t="s">
+        <v>18</v>
+      </c>
+      <c r="C67">
+        <v>2</v>
+      </c>
+      <c r="D67">
+        <v>11</v>
+      </c>
+      <c r="E67" t="s">
+        <v>124</v>
+      </c>
+      <c r="F67" t="s">
+        <v>39</v>
+      </c>
+      <c r="G67" t="s">
+        <v>103</v>
+      </c>
+      <c r="H67" t="s">
+        <v>41</v>
+      </c>
+      <c r="I67" t="s">
+        <v>40</v>
+      </c>
+      <c r="J67">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A68" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B68" t="s">
+        <v>18</v>
+      </c>
+      <c r="C68">
+        <v>2</v>
+      </c>
+      <c r="D68">
+        <v>12</v>
+      </c>
+      <c r="E68" t="s">
+        <v>125</v>
+      </c>
+      <c r="F68" t="s">
+        <v>87</v>
+      </c>
+      <c r="G68" t="s">
+        <v>88</v>
+      </c>
+      <c r="H68" t="s">
+        <v>89</v>
+      </c>
+      <c r="I68" t="s">
+        <v>90</v>
+      </c>
+      <c r="J68">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A69" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B69" t="s">
+        <v>18</v>
+      </c>
+      <c r="C69">
+        <v>2</v>
+      </c>
+      <c r="D69">
+        <v>12</v>
+      </c>
+      <c r="E69" t="s">
+        <v>125</v>
+      </c>
+      <c r="F69" t="s">
+        <v>39</v>
+      </c>
+      <c r="G69" t="s">
+        <v>103</v>
+      </c>
+      <c r="H69" t="s">
+        <v>41</v>
+      </c>
+      <c r="I69" t="s">
+        <v>40</v>
+      </c>
+      <c r="J69">
+        <v>9</v>
+      </c>
+      <c r="L69" t="s">
+        <v>73</v>
+      </c>
+      <c r="M69" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A70" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B70" t="s">
+        <v>18</v>
+      </c>
+      <c r="C70">
+        <v>2</v>
+      </c>
+      <c r="D70">
+        <v>13</v>
+      </c>
+      <c r="E70" t="s">
+        <v>126</v>
+      </c>
+      <c r="F70" t="s">
+        <v>39</v>
+      </c>
+      <c r="G70" t="s">
+        <v>103</v>
+      </c>
+      <c r="H70" t="s">
+        <v>41</v>
+      </c>
+      <c r="I70" t="s">
+        <v>40</v>
+      </c>
+      <c r="J70">
+        <v>12</v>
+      </c>
+      <c r="L70" t="s">
+        <v>73</v>
+      </c>
+      <c r="M70" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A71" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B71" t="s">
+        <v>18</v>
+      </c>
+      <c r="C71">
+        <v>2</v>
+      </c>
+      <c r="D71">
+        <v>14</v>
+      </c>
+      <c r="E71" t="s">
+        <v>128</v>
+      </c>
+      <c r="F71" t="s">
+        <v>20</v>
+      </c>
+      <c r="G71" t="s">
+        <v>21</v>
+      </c>
+      <c r="H71" t="s">
+        <v>24</v>
+      </c>
+      <c r="I71" t="s">
+        <v>23</v>
+      </c>
+      <c r="J71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A72" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B72" t="s">
+        <v>18</v>
+      </c>
+      <c r="C72">
+        <v>2</v>
+      </c>
+      <c r="D72">
+        <v>14</v>
+      </c>
+      <c r="E72" t="s">
+        <v>128</v>
+      </c>
+      <c r="F72" t="s">
+        <v>87</v>
+      </c>
+      <c r="G72" t="s">
+        <v>88</v>
+      </c>
+      <c r="H72" t="s">
+        <v>89</v>
+      </c>
+      <c r="I72" t="s">
+        <v>127</v>
+      </c>
+      <c r="J72">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A73" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B73" t="s">
+        <v>18</v>
+      </c>
+      <c r="C73">
+        <v>2</v>
+      </c>
+      <c r="D73">
+        <v>14</v>
+      </c>
+      <c r="E73" t="s">
+        <v>128</v>
+      </c>
+      <c r="F73" t="s">
+        <v>20</v>
+      </c>
+      <c r="G73" t="s">
+        <v>21</v>
+      </c>
+      <c r="H73" t="s">
+        <v>24</v>
+      </c>
+      <c r="I73" t="s">
+        <v>23</v>
+      </c>
+      <c r="J73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A74" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B74" t="s">
+        <v>18</v>
+      </c>
+      <c r="C74">
+        <v>2</v>
+      </c>
+      <c r="D74">
+        <v>14</v>
+      </c>
+      <c r="E74" t="s">
+        <v>128</v>
+      </c>
+      <c r="F74" t="s">
+        <v>39</v>
+      </c>
+      <c r="G74" t="s">
+        <v>103</v>
+      </c>
+      <c r="H74" t="s">
+        <v>41</v>
+      </c>
+      <c r="I74" t="s">
+        <v>40</v>
+      </c>
+      <c r="J74">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A75" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B75" t="s">
+        <v>18</v>
+      </c>
+      <c r="C75">
+        <v>2</v>
+      </c>
+      <c r="D75">
+        <v>14</v>
+      </c>
+      <c r="E75" t="s">
+        <v>128</v>
+      </c>
+      <c r="F75" t="s">
+        <v>129</v>
+      </c>
+      <c r="G75" t="s">
+        <v>130</v>
+      </c>
+      <c r="H75" t="s">
+        <v>131</v>
+      </c>
+      <c r="I75" t="s">
+        <v>132</v>
+      </c>
+      <c r="J75">
+        <v>2</v>
+      </c>
+      <c r="L75" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A76" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B76" t="s">
+        <v>18</v>
+      </c>
+      <c r="C76">
+        <v>2</v>
+      </c>
+      <c r="D76">
+        <v>15</v>
+      </c>
+      <c r="E76" t="s">
+        <v>133</v>
+      </c>
+      <c r="F76" t="s">
+        <v>39</v>
+      </c>
+      <c r="G76" t="s">
+        <v>103</v>
+      </c>
+      <c r="H76" t="s">
+        <v>41</v>
+      </c>
+      <c r="I76" t="s">
+        <v>40</v>
+      </c>
+      <c r="J76">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A77" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B77" t="s">
+        <v>18</v>
+      </c>
+      <c r="C77">
+        <v>2</v>
+      </c>
+      <c r="D77">
+        <v>16</v>
+      </c>
+      <c r="E77" t="s">
+        <v>134</v>
+      </c>
+      <c r="F77" t="s">
+        <v>87</v>
+      </c>
+      <c r="G77" t="s">
+        <v>108</v>
+      </c>
+      <c r="H77" t="s">
+        <v>89</v>
+      </c>
+      <c r="I77" t="s">
+        <v>90</v>
+      </c>
+      <c r="J77">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A78" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B78" t="s">
+        <v>18</v>
+      </c>
+      <c r="C78">
+        <v>2</v>
+      </c>
+      <c r="D78">
+        <v>16</v>
+      </c>
+      <c r="E78" t="s">
+        <v>134</v>
+      </c>
+      <c r="F78" t="s">
+        <v>46</v>
+      </c>
+      <c r="G78" t="s">
+        <v>21</v>
+      </c>
+      <c r="H78" t="s">
+        <v>48</v>
+      </c>
+      <c r="I78" t="s">
+        <v>135</v>
+      </c>
+      <c r="J78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A79" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B79" t="s">
+        <v>18</v>
+      </c>
+      <c r="C79">
+        <v>2</v>
+      </c>
+      <c r="D79">
+        <v>16</v>
+      </c>
+      <c r="E79" t="s">
+        <v>134</v>
+      </c>
+      <c r="F79" t="s">
+        <v>136</v>
+      </c>
+      <c r="G79" t="s">
+        <v>137</v>
+      </c>
+      <c r="H79" t="s">
+        <v>137</v>
+      </c>
+      <c r="I79" t="s">
+        <v>137</v>
+      </c>
+      <c r="J79">
+        <v>2</v>
+      </c>
+      <c r="M79" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A80" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B80" t="s">
+        <v>18</v>
+      </c>
+      <c r="C80">
+        <v>2</v>
+      </c>
+      <c r="D80">
+        <v>17</v>
+      </c>
+      <c r="E80" t="s">
+        <v>139</v>
+      </c>
+      <c r="F80" t="s">
+        <v>46</v>
+      </c>
+      <c r="G80" t="s">
+        <v>21</v>
+      </c>
+      <c r="H80" t="s">
+        <v>48</v>
+      </c>
+      <c r="I80" t="s">
+        <v>135</v>
+      </c>
+      <c r="J80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A81" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B81" t="s">
+        <v>18</v>
+      </c>
+      <c r="C81">
+        <v>2</v>
+      </c>
+      <c r="D81">
+        <v>17</v>
+      </c>
+      <c r="E81" t="s">
+        <v>139</v>
+      </c>
+      <c r="F81" t="s">
+        <v>136</v>
+      </c>
+      <c r="G81" t="s">
+        <v>137</v>
+      </c>
+      <c r="H81" t="s">
+        <v>137</v>
+      </c>
+      <c r="I81" t="s">
+        <v>137</v>
+      </c>
+      <c r="J81">
+        <v>1</v>
+      </c>
+      <c r="M81" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A82" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B82" t="s">
+        <v>18</v>
+      </c>
+      <c r="C82">
+        <v>2</v>
+      </c>
+      <c r="D82">
+        <v>18</v>
+      </c>
+      <c r="E82" t="s">
+        <v>140</v>
+      </c>
+      <c r="F82" t="s">
+        <v>46</v>
+      </c>
+      <c r="G82" t="s">
+        <v>21</v>
+      </c>
+      <c r="H82" t="s">
+        <v>48</v>
+      </c>
+      <c r="I82" t="s">
+        <v>135</v>
+      </c>
+      <c r="J82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A83" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B83" t="s">
+        <v>18</v>
+      </c>
+      <c r="C83">
+        <v>2</v>
+      </c>
+      <c r="D83">
+        <v>18</v>
+      </c>
+      <c r="E83" t="s">
+        <v>140</v>
+      </c>
+      <c r="F83" t="s">
+        <v>136</v>
+      </c>
+      <c r="G83" t="s">
+        <v>137</v>
+      </c>
+      <c r="H83" t="s">
+        <v>137</v>
+      </c>
+      <c r="I83" t="s">
+        <v>137</v>
+      </c>
+      <c r="J83">
+        <v>1</v>
+      </c>
+      <c r="M83" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated fish survey datasheet
</commit_message>
<xml_diff>
--- a/fishSurveys/data/fishSurveyData.xlsx
+++ b/fishSurveys/data/fishSurveyData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1179" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1740" uniqueCount="267">
   <si>
     <t>date</t>
   </si>
@@ -715,6 +715,108 @@
   </si>
   <si>
     <t xml:space="preserve">Haliocheres sp. </t>
+  </si>
+  <si>
+    <t>GOPR0199.MP4_021.png</t>
+  </si>
+  <si>
+    <t>Haliocheres bivittatus</t>
+  </si>
+  <si>
+    <t>GOPR0199.MP4_022.png</t>
+  </si>
+  <si>
+    <t>GOPR0199.MP4_023.png</t>
+  </si>
+  <si>
+    <t>GOPR0198.MP4_006.png</t>
+  </si>
+  <si>
+    <t>Haemulon charbonarium</t>
+  </si>
+  <si>
+    <t>GOPR0198.MP4_007.png</t>
+  </si>
+  <si>
+    <t>Lujanus apodus</t>
+  </si>
+  <si>
+    <t>GOPR0198.MP4_008.png</t>
+  </si>
+  <si>
+    <t>GOPR0198.MP4_009.png</t>
+  </si>
+  <si>
+    <t>GOPR0198.MP4_010.png</t>
+  </si>
+  <si>
+    <t>GOPR0198.MP4_011.png</t>
+  </si>
+  <si>
+    <t>GOPR0198.MP4_012.png</t>
+  </si>
+  <si>
+    <t>GOPR0198.MP4_013.png</t>
+  </si>
+  <si>
+    <t>GOPR0198.MP4_014.png</t>
+  </si>
+  <si>
+    <t>GOPR0198.MP4_015.png</t>
+  </si>
+  <si>
+    <t>GOPR0198.MP4_016.png</t>
+  </si>
+  <si>
+    <t>GOPR0198.MP4_017.png</t>
+  </si>
+  <si>
+    <t>GOPR0198.MP4_018.png</t>
+  </si>
+  <si>
+    <t>Scarus taeniopterus</t>
+  </si>
+  <si>
+    <t>GOPR0198.MP4_019.png</t>
+  </si>
+  <si>
+    <t>Doctorfish</t>
+  </si>
+  <si>
+    <t>chirurgus</t>
+  </si>
+  <si>
+    <t>Acanthurus chirurgus</t>
+  </si>
+  <si>
+    <t>GOPR0198.MP4_020.png</t>
+  </si>
+  <si>
+    <t>GOPR0198.MP4_021.png</t>
+  </si>
+  <si>
+    <t>Princess Parrotfish</t>
+  </si>
+  <si>
+    <t>Striped Parrotfish</t>
+  </si>
+  <si>
+    <t>GOPR0198.MP4_022.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scarus </t>
+  </si>
+  <si>
+    <t>GOPR0198.MP4_023.png</t>
+  </si>
+  <si>
+    <t>GOPR0198.MP4_024.png</t>
+  </si>
+  <si>
+    <t>GOPR0198.MP4_025.png</t>
+  </si>
+  <si>
+    <t>GOPR0198.MP4_026.png</t>
   </si>
 </sst>
 </file>
@@ -1065,11 +1167,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W193"/>
+  <dimension ref="A1:W267"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A177" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L196" sqref="L196"/>
+      <pane ySplit="1" topLeftCell="A257" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A264" sqref="A264:E267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7049,13 +7151,28 @@
         <v>40</v>
       </c>
       <c r="J179">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L179" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="180" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A180" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B180" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C180" s="4">
+        <v>1</v>
+      </c>
+      <c r="D180">
+        <v>15</v>
+      </c>
+      <c r="E180" t="s">
+        <v>227</v>
+      </c>
       <c r="F180" t="s">
         <v>87</v>
       </c>
@@ -7073,6 +7190,21 @@
       </c>
     </row>
     <row r="181" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A181" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B181" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C181" s="4">
+        <v>1</v>
+      </c>
+      <c r="D181">
+        <v>15</v>
+      </c>
+      <c r="E181" t="s">
+        <v>227</v>
+      </c>
       <c r="F181" t="s">
         <v>224</v>
       </c>
@@ -7093,6 +7225,21 @@
       </c>
     </row>
     <row r="182" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A182" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B182" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C182" s="4">
+        <v>1</v>
+      </c>
+      <c r="D182">
+        <v>15</v>
+      </c>
+      <c r="E182" t="s">
+        <v>227</v>
+      </c>
       <c r="F182" t="s">
         <v>220</v>
       </c>
@@ -7109,7 +7256,375 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="11:15" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A183" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B183" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C183" s="4">
+        <v>1</v>
+      </c>
+      <c r="D183">
+        <v>15</v>
+      </c>
+      <c r="E183" t="s">
+        <v>227</v>
+      </c>
+      <c r="F183" t="s">
+        <v>39</v>
+      </c>
+      <c r="G183" t="s">
+        <v>103</v>
+      </c>
+      <c r="H183" t="s">
+        <v>41</v>
+      </c>
+      <c r="I183" t="s">
+        <v>40</v>
+      </c>
+      <c r="J183">
+        <v>7</v>
+      </c>
+      <c r="L183" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="184" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A184" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B184" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C184" s="4">
+        <v>1</v>
+      </c>
+      <c r="D184">
+        <v>16</v>
+      </c>
+      <c r="E184" t="s">
+        <v>233</v>
+      </c>
+      <c r="F184" t="s">
+        <v>39</v>
+      </c>
+      <c r="G184" t="s">
+        <v>103</v>
+      </c>
+      <c r="H184" t="s">
+        <v>41</v>
+      </c>
+      <c r="I184" t="s">
+        <v>40</v>
+      </c>
+      <c r="J184">
+        <v>5</v>
+      </c>
+      <c r="L184" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A185" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B185" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C185" s="4">
+        <v>1</v>
+      </c>
+      <c r="D185">
+        <v>16</v>
+      </c>
+      <c r="E185" t="s">
+        <v>233</v>
+      </c>
+      <c r="F185" t="s">
+        <v>39</v>
+      </c>
+      <c r="G185" t="s">
+        <v>103</v>
+      </c>
+      <c r="H185" t="s">
+        <v>41</v>
+      </c>
+      <c r="I185" t="s">
+        <v>40</v>
+      </c>
+      <c r="J185">
+        <v>1</v>
+      </c>
+      <c r="L185" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A186" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B186" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C186" s="4">
+        <v>1</v>
+      </c>
+      <c r="D186">
+        <v>16</v>
+      </c>
+      <c r="E186" t="s">
+        <v>233</v>
+      </c>
+      <c r="F186" t="s">
+        <v>220</v>
+      </c>
+      <c r="G186" t="s">
+        <v>81</v>
+      </c>
+      <c r="H186" t="s">
+        <v>221</v>
+      </c>
+      <c r="I186" t="s">
+        <v>222</v>
+      </c>
+      <c r="J186">
+        <v>3</v>
+      </c>
+      <c r="L186" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A187" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B187" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C187" s="4">
+        <v>1</v>
+      </c>
+      <c r="D187">
+        <v>16</v>
+      </c>
+      <c r="E187" t="s">
+        <v>233</v>
+      </c>
+      <c r="F187" t="s">
+        <v>230</v>
+      </c>
+      <c r="G187" t="s">
+        <v>231</v>
+      </c>
+      <c r="H187" t="s">
+        <v>210</v>
+      </c>
+      <c r="I187" t="s">
+        <v>232</v>
+      </c>
+      <c r="J187">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A188" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B188" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C188" s="4">
+        <v>1</v>
+      </c>
+      <c r="D188">
+        <v>16</v>
+      </c>
+      <c r="E188" t="s">
+        <v>233</v>
+      </c>
+      <c r="F188" t="s">
+        <v>129</v>
+      </c>
+      <c r="G188" t="s">
+        <v>231</v>
+      </c>
+      <c r="H188" t="s">
+        <v>131</v>
+      </c>
+      <c r="I188" t="s">
+        <v>234</v>
+      </c>
+      <c r="J188">
+        <v>3</v>
+      </c>
+      <c r="L188" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A189" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B189" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C189" s="4">
+        <v>1</v>
+      </c>
+      <c r="D189">
+        <v>16</v>
+      </c>
+      <c r="E189" t="s">
+        <v>233</v>
+      </c>
+      <c r="F189" t="s">
+        <v>174</v>
+      </c>
+      <c r="G189" t="s">
+        <v>175</v>
+      </c>
+      <c r="H189" t="s">
+        <v>176</v>
+      </c>
+      <c r="I189" t="s">
+        <v>177</v>
+      </c>
+      <c r="J189">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A190" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B190" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C190" s="4">
+        <v>1</v>
+      </c>
+      <c r="D190">
+        <v>17</v>
+      </c>
+      <c r="E190" t="s">
+        <v>235</v>
+      </c>
+      <c r="F190" t="s">
+        <v>174</v>
+      </c>
+      <c r="G190" t="s">
+        <v>175</v>
+      </c>
+      <c r="H190" t="s">
+        <v>176</v>
+      </c>
+      <c r="I190" t="s">
+        <v>177</v>
+      </c>
+      <c r="J190">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A191" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B191" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C191" s="4">
+        <v>1</v>
+      </c>
+      <c r="D191">
+        <v>18</v>
+      </c>
+      <c r="E191" t="s">
+        <v>236</v>
+      </c>
+      <c r="F191" t="s">
+        <v>174</v>
+      </c>
+      <c r="G191" t="s">
+        <v>175</v>
+      </c>
+      <c r="H191" t="s">
+        <v>176</v>
+      </c>
+      <c r="I191" t="s">
+        <v>177</v>
+      </c>
+      <c r="J191">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A192" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B192" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C192" s="4">
+        <v>2</v>
+      </c>
+      <c r="D192">
+        <v>1</v>
+      </c>
+      <c r="E192" t="s">
+        <v>237</v>
+      </c>
+      <c r="F192" t="s">
+        <v>39</v>
+      </c>
+      <c r="G192" t="s">
+        <v>103</v>
+      </c>
+      <c r="H192" t="s">
+        <v>41</v>
+      </c>
+      <c r="I192" t="s">
+        <v>40</v>
+      </c>
+      <c r="J192">
+        <v>2</v>
+      </c>
+      <c r="L192" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="193" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A193" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B193" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C193" s="4">
+        <v>2</v>
+      </c>
+      <c r="D193">
+        <v>1</v>
+      </c>
+      <c r="E193" t="s">
+        <v>237</v>
+      </c>
+      <c r="F193" t="s">
+        <v>25</v>
+      </c>
+      <c r="G193" t="s">
+        <v>47</v>
+      </c>
+      <c r="H193" t="s">
+        <v>26</v>
+      </c>
+      <c r="I193" t="s">
+        <v>27</v>
+      </c>
+      <c r="J193">
+        <v>4</v>
+      </c>
       <c r="K193" s="8"/>
       <c r="L193" s="8"/>
       <c r="M193" s="8"/>
@@ -7117,6 +7632,2491 @@
         <v>232</v>
       </c>
       <c r="O193" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A194" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B194" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C194" s="4">
+        <v>2</v>
+      </c>
+      <c r="D194">
+        <v>1</v>
+      </c>
+      <c r="E194" t="s">
+        <v>237</v>
+      </c>
+      <c r="F194" t="s">
+        <v>190</v>
+      </c>
+      <c r="G194" t="s">
+        <v>150</v>
+      </c>
+      <c r="H194" t="s">
+        <v>192</v>
+      </c>
+      <c r="I194" t="s">
+        <v>191</v>
+      </c>
+      <c r="J194">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="195" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A195" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B195" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C195" s="4">
+        <v>2</v>
+      </c>
+      <c r="D195">
+        <v>1</v>
+      </c>
+      <c r="E195" t="s">
+        <v>237</v>
+      </c>
+      <c r="F195" t="s">
+        <v>146</v>
+      </c>
+      <c r="G195" t="s">
+        <v>21</v>
+      </c>
+      <c r="H195" t="s">
+        <v>147</v>
+      </c>
+      <c r="I195" t="s">
+        <v>148</v>
+      </c>
+      <c r="J195">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="196" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A196" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B196" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C196" s="4">
+        <v>2</v>
+      </c>
+      <c r="D196">
+        <v>1</v>
+      </c>
+      <c r="E196" t="s">
+        <v>237</v>
+      </c>
+      <c r="F196" t="s">
+        <v>51</v>
+      </c>
+      <c r="G196" t="s">
+        <v>21</v>
+      </c>
+      <c r="H196" t="s">
+        <v>52</v>
+      </c>
+      <c r="I196" t="s">
+        <v>238</v>
+      </c>
+      <c r="J196">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A197" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B197" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C197" s="4">
+        <v>2</v>
+      </c>
+      <c r="D197">
+        <v>1</v>
+      </c>
+      <c r="E197" t="s">
+        <v>237</v>
+      </c>
+      <c r="F197" t="s">
+        <v>29</v>
+      </c>
+      <c r="G197" t="s">
+        <v>31</v>
+      </c>
+      <c r="H197" t="s">
+        <v>28</v>
+      </c>
+      <c r="I197" t="s">
+        <v>30</v>
+      </c>
+      <c r="J197">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A198" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B198" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C198" s="4">
+        <v>2</v>
+      </c>
+      <c r="D198">
+        <v>2</v>
+      </c>
+      <c r="E198" t="s">
+        <v>239</v>
+      </c>
+      <c r="F198" t="s">
+        <v>25</v>
+      </c>
+      <c r="G198" t="s">
+        <v>21</v>
+      </c>
+      <c r="H198" t="s">
+        <v>26</v>
+      </c>
+      <c r="I198" t="s">
+        <v>27</v>
+      </c>
+      <c r="J198">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="199" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A199" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B199" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C199" s="4">
+        <v>2</v>
+      </c>
+      <c r="D199">
+        <v>2</v>
+      </c>
+      <c r="E199" t="s">
+        <v>239</v>
+      </c>
+      <c r="F199" t="s">
+        <v>146</v>
+      </c>
+      <c r="G199" t="s">
+        <v>21</v>
+      </c>
+      <c r="H199" t="s">
+        <v>147</v>
+      </c>
+      <c r="I199" t="s">
+        <v>148</v>
+      </c>
+      <c r="J199">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="200" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A200" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B200" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C200" s="4">
+        <v>2</v>
+      </c>
+      <c r="D200">
+        <v>2</v>
+      </c>
+      <c r="E200" t="s">
+        <v>239</v>
+      </c>
+      <c r="F200" t="s">
+        <v>190</v>
+      </c>
+      <c r="G200" t="s">
+        <v>150</v>
+      </c>
+      <c r="H200" t="s">
+        <v>192</v>
+      </c>
+      <c r="I200" t="s">
+        <v>240</v>
+      </c>
+      <c r="J200">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A201" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B201" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C201" s="4">
+        <v>2</v>
+      </c>
+      <c r="D201">
+        <v>2</v>
+      </c>
+      <c r="E201" t="s">
+        <v>239</v>
+      </c>
+      <c r="F201" t="s">
+        <v>51</v>
+      </c>
+      <c r="G201" t="s">
+        <v>21</v>
+      </c>
+      <c r="H201" t="s">
+        <v>52</v>
+      </c>
+      <c r="I201" t="s">
+        <v>53</v>
+      </c>
+      <c r="J201">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="202" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A202" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B202" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C202" s="4">
+        <v>2</v>
+      </c>
+      <c r="D202">
+        <v>3</v>
+      </c>
+      <c r="E202" t="s">
+        <v>241</v>
+      </c>
+      <c r="F202" t="s">
+        <v>25</v>
+      </c>
+      <c r="G202" t="s">
+        <v>21</v>
+      </c>
+      <c r="H202" t="s">
+        <v>26</v>
+      </c>
+      <c r="I202" t="s">
+        <v>27</v>
+      </c>
+      <c r="J202">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="203" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A203" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B203" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C203" s="4">
+        <v>2</v>
+      </c>
+      <c r="D203">
+        <v>3</v>
+      </c>
+      <c r="E203" t="s">
+        <v>241</v>
+      </c>
+      <c r="F203" t="s">
+        <v>146</v>
+      </c>
+      <c r="G203" t="s">
+        <v>21</v>
+      </c>
+      <c r="H203" t="s">
+        <v>147</v>
+      </c>
+      <c r="I203" t="s">
+        <v>148</v>
+      </c>
+      <c r="J203">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="204" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A204" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B204" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C204" s="4">
+        <v>2</v>
+      </c>
+      <c r="D204">
+        <v>3</v>
+      </c>
+      <c r="E204" t="s">
+        <v>241</v>
+      </c>
+      <c r="F204" t="s">
+        <v>51</v>
+      </c>
+      <c r="G204" t="s">
+        <v>21</v>
+      </c>
+      <c r="H204" t="s">
+        <v>52</v>
+      </c>
+      <c r="I204" t="s">
+        <v>53</v>
+      </c>
+      <c r="J204">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="205" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A205" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B205" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C205" s="4">
+        <v>2</v>
+      </c>
+      <c r="D205">
+        <v>3</v>
+      </c>
+      <c r="E205" t="s">
+        <v>241</v>
+      </c>
+      <c r="F205" t="s">
+        <v>190</v>
+      </c>
+      <c r="G205" t="s">
+        <v>150</v>
+      </c>
+      <c r="H205" t="s">
+        <v>192</v>
+      </c>
+      <c r="I205" t="s">
+        <v>191</v>
+      </c>
+      <c r="J205">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="206" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A206" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B206" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C206" s="4">
+        <v>2</v>
+      </c>
+      <c r="D206">
+        <v>3</v>
+      </c>
+      <c r="E206" t="s">
+        <v>241</v>
+      </c>
+      <c r="F206" t="s">
+        <v>87</v>
+      </c>
+      <c r="G206" t="s">
+        <v>88</v>
+      </c>
+      <c r="H206" t="s">
+        <v>89</v>
+      </c>
+      <c r="I206" t="s">
+        <v>90</v>
+      </c>
+      <c r="J206">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A207" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B207" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C207" s="4">
+        <v>2</v>
+      </c>
+      <c r="D207">
+        <v>4</v>
+      </c>
+      <c r="E207" t="s">
+        <v>242</v>
+      </c>
+      <c r="F207" t="s">
+        <v>25</v>
+      </c>
+      <c r="G207" t="s">
+        <v>21</v>
+      </c>
+      <c r="H207" t="s">
+        <v>26</v>
+      </c>
+      <c r="I207" t="s">
+        <v>27</v>
+      </c>
+      <c r="J207">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A208" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B208" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C208" s="4">
+        <v>2</v>
+      </c>
+      <c r="D208">
+        <v>4</v>
+      </c>
+      <c r="E208" t="s">
+        <v>242</v>
+      </c>
+      <c r="F208" t="s">
+        <v>51</v>
+      </c>
+      <c r="G208" t="s">
+        <v>21</v>
+      </c>
+      <c r="H208" t="s">
+        <v>52</v>
+      </c>
+      <c r="I208" t="s">
+        <v>53</v>
+      </c>
+      <c r="J208">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="209" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A209" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B209" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C209" s="4">
+        <v>2</v>
+      </c>
+      <c r="D209">
+        <v>4</v>
+      </c>
+      <c r="E209" t="s">
+        <v>242</v>
+      </c>
+      <c r="F209" t="s">
+        <v>146</v>
+      </c>
+      <c r="G209" t="s">
+        <v>21</v>
+      </c>
+      <c r="H209" t="s">
+        <v>147</v>
+      </c>
+      <c r="I209" t="s">
+        <v>148</v>
+      </c>
+      <c r="J209">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A210" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B210" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C210" s="4">
+        <v>2</v>
+      </c>
+      <c r="D210">
+        <v>5</v>
+      </c>
+      <c r="E210" t="s">
+        <v>243</v>
+      </c>
+      <c r="F210" t="s">
+        <v>51</v>
+      </c>
+      <c r="G210" t="s">
+        <v>21</v>
+      </c>
+      <c r="H210" t="s">
+        <v>52</v>
+      </c>
+      <c r="I210" t="s">
+        <v>53</v>
+      </c>
+      <c r="J210">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A211" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B211" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C211" s="4">
+        <v>2</v>
+      </c>
+      <c r="D211">
+        <v>5</v>
+      </c>
+      <c r="E211" t="s">
+        <v>243</v>
+      </c>
+      <c r="F211" t="s">
+        <v>39</v>
+      </c>
+      <c r="G211" t="s">
+        <v>103</v>
+      </c>
+      <c r="H211" t="s">
+        <v>41</v>
+      </c>
+      <c r="I211" t="s">
+        <v>40</v>
+      </c>
+      <c r="J211">
+        <v>1</v>
+      </c>
+      <c r="K211" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="212" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A212" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B212" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C212" s="4">
+        <v>2</v>
+      </c>
+      <c r="D212">
+        <v>6</v>
+      </c>
+      <c r="E212" t="s">
+        <v>244</v>
+      </c>
+      <c r="F212" t="s">
+        <v>39</v>
+      </c>
+      <c r="G212" t="s">
+        <v>103</v>
+      </c>
+      <c r="H212" t="s">
+        <v>41</v>
+      </c>
+      <c r="I212" t="s">
+        <v>40</v>
+      </c>
+      <c r="J212">
+        <v>1</v>
+      </c>
+      <c r="K212" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="213" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A213" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B213" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C213" s="4">
+        <v>2</v>
+      </c>
+      <c r="D213">
+        <v>6</v>
+      </c>
+      <c r="E213" t="s">
+        <v>244</v>
+      </c>
+      <c r="F213" t="s">
+        <v>87</v>
+      </c>
+      <c r="G213" t="s">
+        <v>88</v>
+      </c>
+      <c r="H213" t="s">
+        <v>89</v>
+      </c>
+      <c r="I213" t="s">
+        <v>90</v>
+      </c>
+      <c r="J213">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="214" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A214" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B214" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C214" s="4">
+        <v>2</v>
+      </c>
+      <c r="D214">
+        <v>6</v>
+      </c>
+      <c r="E214" t="s">
+        <v>244</v>
+      </c>
+      <c r="F214" t="s">
+        <v>51</v>
+      </c>
+      <c r="G214" t="s">
+        <v>21</v>
+      </c>
+      <c r="H214" t="s">
+        <v>52</v>
+      </c>
+      <c r="I214" t="s">
+        <v>53</v>
+      </c>
+      <c r="J214">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A215" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B215" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C215" s="4">
+        <v>2</v>
+      </c>
+      <c r="D215">
+        <v>7</v>
+      </c>
+      <c r="E215" t="s">
+        <v>245</v>
+      </c>
+      <c r="F215" t="s">
+        <v>39</v>
+      </c>
+      <c r="G215" t="s">
+        <v>103</v>
+      </c>
+      <c r="H215" t="s">
+        <v>41</v>
+      </c>
+      <c r="I215" t="s">
+        <v>40</v>
+      </c>
+      <c r="J215">
+        <v>17</v>
+      </c>
+      <c r="K215" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="216" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A216" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B216" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C216" s="4">
+        <v>2</v>
+      </c>
+      <c r="D216">
+        <v>7</v>
+      </c>
+      <c r="E216" t="s">
+        <v>245</v>
+      </c>
+      <c r="F216" t="s">
+        <v>113</v>
+      </c>
+      <c r="G216" t="s">
+        <v>33</v>
+      </c>
+      <c r="H216" t="s">
+        <v>114</v>
+      </c>
+      <c r="I216" t="s">
+        <v>115</v>
+      </c>
+      <c r="J216">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="217" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A217" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B217" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C217" s="4">
+        <v>2</v>
+      </c>
+      <c r="D217">
+        <v>7</v>
+      </c>
+      <c r="E217" t="s">
+        <v>245</v>
+      </c>
+      <c r="F217" t="s">
+        <v>87</v>
+      </c>
+      <c r="G217" t="s">
+        <v>88</v>
+      </c>
+      <c r="H217" t="s">
+        <v>89</v>
+      </c>
+      <c r="I217" t="s">
+        <v>90</v>
+      </c>
+      <c r="J217">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="218" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A218" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B218" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C218" s="4">
+        <v>2</v>
+      </c>
+      <c r="D218">
+        <v>8</v>
+      </c>
+      <c r="E218" t="s">
+        <v>246</v>
+      </c>
+      <c r="F218" t="s">
+        <v>39</v>
+      </c>
+      <c r="G218" t="s">
+        <v>103</v>
+      </c>
+      <c r="H218" t="s">
+        <v>41</v>
+      </c>
+      <c r="I218" t="s">
+        <v>40</v>
+      </c>
+      <c r="J218">
+        <v>11</v>
+      </c>
+      <c r="K218" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="219" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A219" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B219" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C219" s="4">
+        <v>2</v>
+      </c>
+      <c r="D219">
+        <v>9</v>
+      </c>
+      <c r="E219" t="s">
+        <v>247</v>
+      </c>
+      <c r="F219" t="s">
+        <v>39</v>
+      </c>
+      <c r="G219" t="s">
+        <v>42</v>
+      </c>
+      <c r="H219" t="s">
+        <v>41</v>
+      </c>
+      <c r="I219" t="s">
+        <v>40</v>
+      </c>
+      <c r="J219">
+        <v>16</v>
+      </c>
+      <c r="K219" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="220" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A220" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B220" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C220" s="4">
+        <v>2</v>
+      </c>
+      <c r="D220">
+        <v>9</v>
+      </c>
+      <c r="E220" t="s">
+        <v>247</v>
+      </c>
+      <c r="F220" t="s">
+        <v>87</v>
+      </c>
+      <c r="G220" t="s">
+        <v>88</v>
+      </c>
+      <c r="H220" t="s">
+        <v>89</v>
+      </c>
+      <c r="I220" t="s">
+        <v>90</v>
+      </c>
+      <c r="J220">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="221" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A221" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B221" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C221" s="4">
+        <v>2</v>
+      </c>
+      <c r="D221">
+        <v>10</v>
+      </c>
+      <c r="E221" t="s">
+        <v>248</v>
+      </c>
+      <c r="F221" t="s">
+        <v>87</v>
+      </c>
+      <c r="G221" t="s">
+        <v>108</v>
+      </c>
+      <c r="H221" t="s">
+        <v>89</v>
+      </c>
+      <c r="I221" t="s">
+        <v>90</v>
+      </c>
+      <c r="J221">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="222" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A222" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B222" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C222" s="4">
+        <v>2</v>
+      </c>
+      <c r="D222">
+        <v>10</v>
+      </c>
+      <c r="E222" t="s">
+        <v>248</v>
+      </c>
+      <c r="F222" t="s">
+        <v>39</v>
+      </c>
+      <c r="G222" t="s">
+        <v>103</v>
+      </c>
+      <c r="H222" t="s">
+        <v>41</v>
+      </c>
+      <c r="I222" t="s">
+        <v>40</v>
+      </c>
+      <c r="J222">
+        <v>3</v>
+      </c>
+      <c r="K222" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="223" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A223" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B223" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C223" s="4">
+        <v>2</v>
+      </c>
+      <c r="D223">
+        <v>11</v>
+      </c>
+      <c r="E223" t="s">
+        <v>249</v>
+      </c>
+      <c r="F223" t="s">
+        <v>39</v>
+      </c>
+      <c r="G223" t="s">
+        <v>103</v>
+      </c>
+      <c r="H223" t="s">
+        <v>41</v>
+      </c>
+      <c r="I223" t="s">
+        <v>40</v>
+      </c>
+      <c r="J223">
+        <v>3</v>
+      </c>
+      <c r="K223" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="224" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A224" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B224" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C224" s="4">
+        <v>2</v>
+      </c>
+      <c r="D224">
+        <v>12</v>
+      </c>
+      <c r="E224" t="s">
+        <v>250</v>
+      </c>
+      <c r="F224" t="s">
+        <v>39</v>
+      </c>
+      <c r="G224" t="s">
+        <v>103</v>
+      </c>
+      <c r="H224" t="s">
+        <v>41</v>
+      </c>
+      <c r="I224" t="s">
+        <v>40</v>
+      </c>
+      <c r="J224">
+        <v>5</v>
+      </c>
+      <c r="K224" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="225" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A225" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B225" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C225" s="4">
+        <v>2</v>
+      </c>
+      <c r="D225">
+        <v>12</v>
+      </c>
+      <c r="E225" t="s">
+        <v>250</v>
+      </c>
+      <c r="F225" t="s">
+        <v>87</v>
+      </c>
+      <c r="G225" t="s">
+        <v>88</v>
+      </c>
+      <c r="H225" t="s">
+        <v>89</v>
+      </c>
+      <c r="I225" t="s">
+        <v>90</v>
+      </c>
+      <c r="J225">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="226" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A226" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B226" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C226" s="4">
+        <v>2</v>
+      </c>
+      <c r="D226">
+        <v>13</v>
+      </c>
+      <c r="E226" t="s">
+        <v>251</v>
+      </c>
+      <c r="F226" t="s">
+        <v>39</v>
+      </c>
+      <c r="G226" t="s">
+        <v>103</v>
+      </c>
+      <c r="H226" t="s">
+        <v>41</v>
+      </c>
+      <c r="I226" t="s">
+        <v>40</v>
+      </c>
+      <c r="J226">
+        <v>2</v>
+      </c>
+      <c r="K226" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="227" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A227" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B227" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C227" s="4">
+        <v>2</v>
+      </c>
+      <c r="D227">
+        <v>13</v>
+      </c>
+      <c r="E227" t="s">
+        <v>251</v>
+      </c>
+      <c r="F227" t="s">
+        <v>259</v>
+      </c>
+      <c r="G227" t="s">
+        <v>81</v>
+      </c>
+      <c r="H227" t="s">
+        <v>221</v>
+      </c>
+      <c r="I227" t="s">
+        <v>252</v>
+      </c>
+      <c r="J227">
+        <v>2</v>
+      </c>
+      <c r="K227" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="228" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A228" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B228" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C228" s="4">
+        <v>2</v>
+      </c>
+      <c r="D228">
+        <v>14</v>
+      </c>
+      <c r="E228" t="s">
+        <v>253</v>
+      </c>
+      <c r="F228" t="s">
+        <v>39</v>
+      </c>
+      <c r="G228" t="s">
+        <v>103</v>
+      </c>
+      <c r="H228" t="s">
+        <v>41</v>
+      </c>
+      <c r="I228" t="s">
+        <v>40</v>
+      </c>
+      <c r="J228">
+        <v>9</v>
+      </c>
+      <c r="K228" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="229" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A229" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B229" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C229" s="4">
+        <v>2</v>
+      </c>
+      <c r="D229">
+        <v>14</v>
+      </c>
+      <c r="E229" t="s">
+        <v>253</v>
+      </c>
+      <c r="F229" t="s">
+        <v>259</v>
+      </c>
+      <c r="G229" t="s">
+        <v>81</v>
+      </c>
+      <c r="H229" t="s">
+        <v>221</v>
+      </c>
+      <c r="I229" t="s">
+        <v>252</v>
+      </c>
+      <c r="J229">
+        <v>2</v>
+      </c>
+      <c r="K229" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="230" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A230" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B230" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C230" s="4">
+        <v>2</v>
+      </c>
+      <c r="D230">
+        <v>14</v>
+      </c>
+      <c r="E230" t="s">
+        <v>253</v>
+      </c>
+      <c r="F230" t="s">
+        <v>254</v>
+      </c>
+      <c r="G230" t="s">
+        <v>175</v>
+      </c>
+      <c r="H230" t="s">
+        <v>255</v>
+      </c>
+      <c r="I230" t="s">
+        <v>256</v>
+      </c>
+      <c r="J230">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="231" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A231" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B231" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C231" s="4">
+        <v>2</v>
+      </c>
+      <c r="D231">
+        <v>15</v>
+      </c>
+      <c r="E231" t="s">
+        <v>257</v>
+      </c>
+      <c r="F231" t="s">
+        <v>259</v>
+      </c>
+      <c r="G231" t="s">
+        <v>81</v>
+      </c>
+      <c r="H231" t="s">
+        <v>221</v>
+      </c>
+      <c r="I231" t="s">
+        <v>252</v>
+      </c>
+      <c r="J231">
+        <v>2</v>
+      </c>
+      <c r="K231" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="232" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A232" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B232" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C232" s="4">
+        <v>2</v>
+      </c>
+      <c r="D232">
+        <v>15</v>
+      </c>
+      <c r="E232" t="s">
+        <v>257</v>
+      </c>
+      <c r="F232" t="s">
+        <v>39</v>
+      </c>
+      <c r="G232" t="s">
+        <v>103</v>
+      </c>
+      <c r="H232" t="s">
+        <v>41</v>
+      </c>
+      <c r="I232" t="s">
+        <v>40</v>
+      </c>
+      <c r="J232">
+        <v>1</v>
+      </c>
+      <c r="K232" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="233" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A233" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B233" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C233" s="4">
+        <v>2</v>
+      </c>
+      <c r="D233">
+        <v>15</v>
+      </c>
+      <c r="E233" t="s">
+        <v>257</v>
+      </c>
+      <c r="F233" t="s">
+        <v>39</v>
+      </c>
+      <c r="G233" t="s">
+        <v>103</v>
+      </c>
+      <c r="H233" t="s">
+        <v>41</v>
+      </c>
+      <c r="I233" t="s">
+        <v>40</v>
+      </c>
+      <c r="J233">
+        <v>12</v>
+      </c>
+      <c r="K233" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="234" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A234" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B234" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C234" s="4">
+        <v>2</v>
+      </c>
+      <c r="D234">
+        <v>15</v>
+      </c>
+      <c r="E234" t="s">
+        <v>257</v>
+      </c>
+      <c r="F234" t="s">
+        <v>51</v>
+      </c>
+      <c r="G234" t="s">
+        <v>21</v>
+      </c>
+      <c r="H234" t="s">
+        <v>52</v>
+      </c>
+      <c r="I234" t="s">
+        <v>53</v>
+      </c>
+      <c r="J234">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="235" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A235" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B235" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C235" s="4">
+        <v>2</v>
+      </c>
+      <c r="D235">
+        <v>15</v>
+      </c>
+      <c r="E235" t="s">
+        <v>257</v>
+      </c>
+      <c r="F235" t="s">
+        <v>87</v>
+      </c>
+      <c r="G235" t="s">
+        <v>88</v>
+      </c>
+      <c r="H235" t="s">
+        <v>89</v>
+      </c>
+      <c r="I235" t="s">
+        <v>90</v>
+      </c>
+      <c r="J235">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="236" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A236" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B236" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C236" s="4">
+        <v>2</v>
+      </c>
+      <c r="D236">
+        <v>15</v>
+      </c>
+      <c r="E236" t="s">
+        <v>257</v>
+      </c>
+      <c r="F236" t="s">
+        <v>129</v>
+      </c>
+      <c r="G236" t="s">
+        <v>231</v>
+      </c>
+      <c r="H236" t="s">
+        <v>131</v>
+      </c>
+      <c r="I236" t="s">
+        <v>234</v>
+      </c>
+      <c r="J236">
+        <v>1</v>
+      </c>
+      <c r="K236" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="237" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A237" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B237" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C237" s="4">
+        <v>2</v>
+      </c>
+      <c r="D237">
+        <v>15</v>
+      </c>
+      <c r="E237" t="s">
+        <v>257</v>
+      </c>
+      <c r="F237" t="s">
+        <v>254</v>
+      </c>
+      <c r="G237" t="s">
+        <v>175</v>
+      </c>
+      <c r="H237" t="s">
+        <v>255</v>
+      </c>
+      <c r="I237" t="s">
+        <v>256</v>
+      </c>
+      <c r="J237">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="238" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A238" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B238" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C238" s="4">
+        <v>2</v>
+      </c>
+      <c r="D238">
+        <v>16</v>
+      </c>
+      <c r="E238" t="s">
+        <v>258</v>
+      </c>
+      <c r="F238" t="s">
+        <v>39</v>
+      </c>
+      <c r="G238" t="s">
+        <v>103</v>
+      </c>
+      <c r="H238" t="s">
+        <v>41</v>
+      </c>
+      <c r="I238" t="s">
+        <v>40</v>
+      </c>
+      <c r="J238">
+        <v>10</v>
+      </c>
+      <c r="K238" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="239" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A239" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B239" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C239" s="4">
+        <v>2</v>
+      </c>
+      <c r="D239">
+        <v>16</v>
+      </c>
+      <c r="E239" t="s">
+        <v>258</v>
+      </c>
+      <c r="F239" t="s">
+        <v>259</v>
+      </c>
+      <c r="G239" t="s">
+        <v>81</v>
+      </c>
+      <c r="H239" t="s">
+        <v>221</v>
+      </c>
+      <c r="I239" t="s">
+        <v>252</v>
+      </c>
+      <c r="J239">
+        <v>2</v>
+      </c>
+      <c r="K239" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="240" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A240" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B240" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C240" s="4">
+        <v>2</v>
+      </c>
+      <c r="D240">
+        <v>16</v>
+      </c>
+      <c r="E240" t="s">
+        <v>258</v>
+      </c>
+      <c r="F240" t="s">
+        <v>260</v>
+      </c>
+      <c r="G240" t="s">
+        <v>81</v>
+      </c>
+      <c r="H240" t="s">
+        <v>82</v>
+      </c>
+      <c r="I240" t="s">
+        <v>83</v>
+      </c>
+      <c r="J240">
+        <v>2</v>
+      </c>
+      <c r="K240" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="241" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A241" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B241" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C241" s="4">
+        <v>2</v>
+      </c>
+      <c r="D241">
+        <v>17</v>
+      </c>
+      <c r="E241" t="s">
+        <v>261</v>
+      </c>
+      <c r="F241" t="s">
+        <v>259</v>
+      </c>
+      <c r="G241" t="s">
+        <v>262</v>
+      </c>
+      <c r="H241" t="s">
+        <v>221</v>
+      </c>
+      <c r="I241" t="s">
+        <v>252</v>
+      </c>
+      <c r="J241">
+        <v>3</v>
+      </c>
+      <c r="K241" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="242" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A242" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B242" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C242" s="4">
+        <v>2</v>
+      </c>
+      <c r="D242">
+        <v>17</v>
+      </c>
+      <c r="E242" t="s">
+        <v>261</v>
+      </c>
+      <c r="F242" t="s">
+        <v>260</v>
+      </c>
+      <c r="G242" t="s">
+        <v>81</v>
+      </c>
+      <c r="H242" t="s">
+        <v>82</v>
+      </c>
+      <c r="I242" t="s">
+        <v>83</v>
+      </c>
+      <c r="J242">
+        <v>2</v>
+      </c>
+      <c r="K242" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="243" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A243" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B243" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C243" s="4">
+        <v>2</v>
+      </c>
+      <c r="D243">
+        <v>17</v>
+      </c>
+      <c r="E243" t="s">
+        <v>261</v>
+      </c>
+      <c r="F243" t="s">
+        <v>39</v>
+      </c>
+      <c r="G243" t="s">
+        <v>42</v>
+      </c>
+      <c r="H243" t="s">
+        <v>41</v>
+      </c>
+      <c r="I243" t="s">
+        <v>40</v>
+      </c>
+      <c r="J243">
+        <v>8</v>
+      </c>
+      <c r="K243" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="244" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A244" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B244" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C244" s="4">
+        <v>2</v>
+      </c>
+      <c r="D244">
+        <v>17</v>
+      </c>
+      <c r="E244" t="s">
+        <v>261</v>
+      </c>
+      <c r="F244" t="s">
+        <v>129</v>
+      </c>
+      <c r="G244" t="s">
+        <v>231</v>
+      </c>
+      <c r="H244" t="s">
+        <v>131</v>
+      </c>
+      <c r="I244" t="s">
+        <v>234</v>
+      </c>
+      <c r="J244">
+        <v>4</v>
+      </c>
+      <c r="K244" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="245" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A245" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B245" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C245" s="4">
+        <v>2</v>
+      </c>
+      <c r="D245">
+        <v>18</v>
+      </c>
+      <c r="E245" t="s">
+        <v>263</v>
+      </c>
+      <c r="F245" t="s">
+        <v>259</v>
+      </c>
+      <c r="G245" t="s">
+        <v>81</v>
+      </c>
+      <c r="H245" t="s">
+        <v>221</v>
+      </c>
+      <c r="I245" t="s">
+        <v>252</v>
+      </c>
+      <c r="J245">
+        <v>2</v>
+      </c>
+      <c r="K245" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="246" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A246" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B246" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C246" s="4">
+        <v>2</v>
+      </c>
+      <c r="D246">
+        <v>18</v>
+      </c>
+      <c r="E246" t="s">
+        <v>263</v>
+      </c>
+      <c r="F246" t="s">
+        <v>260</v>
+      </c>
+      <c r="G246" t="s">
+        <v>81</v>
+      </c>
+      <c r="H246" t="s">
+        <v>82</v>
+      </c>
+      <c r="I246" t="s">
+        <v>83</v>
+      </c>
+      <c r="J246">
+        <v>2</v>
+      </c>
+      <c r="K246" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="247" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A247" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B247" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C247" s="4">
+        <v>2</v>
+      </c>
+      <c r="D247">
+        <v>18</v>
+      </c>
+      <c r="E247" t="s">
+        <v>263</v>
+      </c>
+      <c r="F247" t="s">
+        <v>129</v>
+      </c>
+      <c r="G247" t="s">
+        <v>231</v>
+      </c>
+      <c r="H247" t="s">
+        <v>131</v>
+      </c>
+      <c r="I247" t="s">
+        <v>234</v>
+      </c>
+      <c r="J247">
+        <v>3</v>
+      </c>
+      <c r="K247" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="248" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A248" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B248" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C248" s="4">
+        <v>2</v>
+      </c>
+      <c r="D248">
+        <v>18</v>
+      </c>
+      <c r="E248" t="s">
+        <v>263</v>
+      </c>
+      <c r="F248" t="s">
+        <v>39</v>
+      </c>
+      <c r="G248" t="s">
+        <v>103</v>
+      </c>
+      <c r="H248" t="s">
+        <v>41</v>
+      </c>
+      <c r="I248" t="s">
+        <v>40</v>
+      </c>
+      <c r="J248">
+        <v>4</v>
+      </c>
+      <c r="K248" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="249" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A249" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B249" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C249" s="4">
+        <v>2</v>
+      </c>
+      <c r="D249">
+        <v>18</v>
+      </c>
+      <c r="E249" t="s">
+        <v>263</v>
+      </c>
+      <c r="F249" t="s">
+        <v>46</v>
+      </c>
+      <c r="G249" t="s">
+        <v>21</v>
+      </c>
+      <c r="H249" t="s">
+        <v>48</v>
+      </c>
+      <c r="I249" t="s">
+        <v>49</v>
+      </c>
+      <c r="J249">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="250" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A250" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B250" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C250" s="4">
+        <v>2</v>
+      </c>
+      <c r="D250">
+        <v>19</v>
+      </c>
+      <c r="E250" t="s">
+        <v>264</v>
+      </c>
+      <c r="F250" t="s">
+        <v>260</v>
+      </c>
+      <c r="G250" t="s">
+        <v>81</v>
+      </c>
+      <c r="H250" t="s">
+        <v>82</v>
+      </c>
+      <c r="I250" t="s">
+        <v>83</v>
+      </c>
+      <c r="J250">
+        <v>2</v>
+      </c>
+      <c r="K250" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="251" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A251" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B251" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C251" s="4">
+        <v>2</v>
+      </c>
+      <c r="D251">
+        <v>19</v>
+      </c>
+      <c r="E251" t="s">
+        <v>264</v>
+      </c>
+      <c r="F251" t="s">
+        <v>259</v>
+      </c>
+      <c r="G251" t="s">
+        <v>81</v>
+      </c>
+      <c r="H251" t="s">
+        <v>221</v>
+      </c>
+      <c r="I251" t="s">
+        <v>252</v>
+      </c>
+      <c r="J251">
+        <v>1</v>
+      </c>
+      <c r="K251" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="252" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A252" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B252" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C252" s="4">
+        <v>2</v>
+      </c>
+      <c r="D252">
+        <v>19</v>
+      </c>
+      <c r="E252" t="s">
+        <v>264</v>
+      </c>
+      <c r="F252" t="s">
+        <v>113</v>
+      </c>
+      <c r="G252" t="s">
+        <v>33</v>
+      </c>
+      <c r="H252" t="s">
+        <v>114</v>
+      </c>
+      <c r="I252" t="s">
+        <v>115</v>
+      </c>
+      <c r="J252">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="253" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A253" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B253" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C253" s="4">
+        <v>2</v>
+      </c>
+      <c r="D253">
+        <v>19</v>
+      </c>
+      <c r="E253" t="s">
+        <v>264</v>
+      </c>
+      <c r="F253" t="s">
+        <v>46</v>
+      </c>
+      <c r="G253" t="s">
+        <v>21</v>
+      </c>
+      <c r="H253" t="s">
+        <v>48</v>
+      </c>
+      <c r="I253" t="s">
+        <v>49</v>
+      </c>
+      <c r="J253">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="254" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A254" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B254" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C254" s="4">
+        <v>2</v>
+      </c>
+      <c r="D254">
+        <v>19</v>
+      </c>
+      <c r="E254" t="s">
+        <v>264</v>
+      </c>
+      <c r="F254" t="s">
+        <v>39</v>
+      </c>
+      <c r="G254" t="s">
+        <v>103</v>
+      </c>
+      <c r="H254" t="s">
+        <v>41</v>
+      </c>
+      <c r="I254" t="s">
+        <v>40</v>
+      </c>
+      <c r="J254">
+        <v>1</v>
+      </c>
+      <c r="K254" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="255" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A255" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B255" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C255" s="4">
+        <v>2</v>
+      </c>
+      <c r="D255">
+        <v>19</v>
+      </c>
+      <c r="E255" t="s">
+        <v>264</v>
+      </c>
+      <c r="F255" t="s">
+        <v>39</v>
+      </c>
+      <c r="G255" t="s">
+        <v>42</v>
+      </c>
+      <c r="H255" t="s">
+        <v>41</v>
+      </c>
+      <c r="I255" t="s">
+        <v>40</v>
+      </c>
+      <c r="J255">
+        <v>4</v>
+      </c>
+      <c r="K255" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="256" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A256" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B256" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C256" s="4">
+        <v>2</v>
+      </c>
+      <c r="D256">
+        <v>19</v>
+      </c>
+      <c r="E256" t="s">
+        <v>264</v>
+      </c>
+      <c r="F256" t="s">
+        <v>87</v>
+      </c>
+      <c r="G256" t="s">
+        <v>88</v>
+      </c>
+      <c r="H256" t="s">
+        <v>89</v>
+      </c>
+      <c r="I256" t="s">
+        <v>90</v>
+      </c>
+      <c r="J256">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="257" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A257" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B257" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C257" s="4">
+        <v>2</v>
+      </c>
+      <c r="D257">
+        <v>20</v>
+      </c>
+      <c r="E257" t="s">
+        <v>265</v>
+      </c>
+      <c r="F257" t="s">
+        <v>259</v>
+      </c>
+      <c r="G257" t="s">
+        <v>81</v>
+      </c>
+      <c r="H257" t="s">
+        <v>221</v>
+      </c>
+      <c r="I257" t="s">
+        <v>252</v>
+      </c>
+      <c r="J257">
+        <v>7</v>
+      </c>
+      <c r="K257" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="258" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A258" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B258" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C258" s="4">
+        <v>2</v>
+      </c>
+      <c r="D258">
+        <v>20</v>
+      </c>
+      <c r="E258" t="s">
+        <v>265</v>
+      </c>
+      <c r="F258" t="s">
+        <v>39</v>
+      </c>
+      <c r="G258" t="s">
+        <v>103</v>
+      </c>
+      <c r="H258" t="s">
+        <v>41</v>
+      </c>
+      <c r="I258" t="s">
+        <v>40</v>
+      </c>
+      <c r="J258">
+        <v>1</v>
+      </c>
+      <c r="K258" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="259" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A259" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B259" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C259" s="4">
+        <v>2</v>
+      </c>
+      <c r="D259">
+        <v>20</v>
+      </c>
+      <c r="E259" t="s">
+        <v>265</v>
+      </c>
+      <c r="F259" t="s">
+        <v>39</v>
+      </c>
+      <c r="G259" t="s">
+        <v>42</v>
+      </c>
+      <c r="H259" t="s">
+        <v>41</v>
+      </c>
+      <c r="I259" t="s">
+        <v>40</v>
+      </c>
+      <c r="J259">
+        <v>5</v>
+      </c>
+      <c r="K259" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="260" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A260" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B260" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C260" s="4">
+        <v>2</v>
+      </c>
+      <c r="D260">
+        <v>20</v>
+      </c>
+      <c r="E260" t="s">
+        <v>265</v>
+      </c>
+      <c r="F260" t="s">
+        <v>129</v>
+      </c>
+      <c r="G260" t="s">
+        <v>231</v>
+      </c>
+      <c r="H260" t="s">
+        <v>131</v>
+      </c>
+      <c r="I260" t="s">
+        <v>234</v>
+      </c>
+      <c r="J260">
+        <v>2</v>
+      </c>
+      <c r="K260" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="261" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A261" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B261" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C261" s="4">
+        <v>2</v>
+      </c>
+      <c r="D261">
+        <v>20</v>
+      </c>
+      <c r="E261" t="s">
+        <v>265</v>
+      </c>
+      <c r="F261" t="s">
+        <v>113</v>
+      </c>
+      <c r="G261" t="s">
+        <v>33</v>
+      </c>
+      <c r="H261" t="s">
+        <v>114</v>
+      </c>
+      <c r="I261" t="s">
+        <v>115</v>
+      </c>
+      <c r="J261">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="262" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A262" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B262" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C262" s="4">
+        <v>2</v>
+      </c>
+      <c r="D262">
+        <v>20</v>
+      </c>
+      <c r="E262" t="s">
+        <v>265</v>
+      </c>
+      <c r="F262" t="s">
+        <v>87</v>
+      </c>
+      <c r="G262" t="s">
+        <v>88</v>
+      </c>
+      <c r="H262" t="s">
+        <v>89</v>
+      </c>
+      <c r="I262" t="s">
+        <v>90</v>
+      </c>
+      <c r="J262">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="263" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A263" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B263" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C263" s="4">
+        <v>2</v>
+      </c>
+      <c r="D263">
+        <v>21</v>
+      </c>
+      <c r="E263" t="s">
+        <v>266</v>
+      </c>
+      <c r="F263" t="s">
+        <v>129</v>
+      </c>
+      <c r="G263" t="s">
+        <v>231</v>
+      </c>
+      <c r="H263" t="s">
+        <v>131</v>
+      </c>
+      <c r="I263" t="s">
+        <v>234</v>
+      </c>
+      <c r="J263">
+        <v>2</v>
+      </c>
+      <c r="K263" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="264" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A264" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B264" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C264" s="4">
+        <v>2</v>
+      </c>
+      <c r="D264">
+        <v>21</v>
+      </c>
+      <c r="E264" t="s">
+        <v>266</v>
+      </c>
+      <c r="F264" t="s">
+        <v>259</v>
+      </c>
+      <c r="G264" t="s">
+        <v>81</v>
+      </c>
+      <c r="H264" t="s">
+        <v>221</v>
+      </c>
+      <c r="I264" t="s">
+        <v>252</v>
+      </c>
+      <c r="J264">
+        <v>6</v>
+      </c>
+      <c r="K264" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="265" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A265" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B265" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C265" s="4">
+        <v>2</v>
+      </c>
+      <c r="D265">
+        <v>21</v>
+      </c>
+      <c r="E265" t="s">
+        <v>266</v>
+      </c>
+      <c r="F265" t="s">
+        <v>39</v>
+      </c>
+      <c r="G265" t="s">
+        <v>103</v>
+      </c>
+      <c r="H265" t="s">
+        <v>41</v>
+      </c>
+      <c r="I265" t="s">
+        <v>40</v>
+      </c>
+      <c r="J265">
+        <v>1</v>
+      </c>
+      <c r="K265" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="266" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A266" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B266" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C266" s="4">
+        <v>2</v>
+      </c>
+      <c r="D266">
+        <v>21</v>
+      </c>
+      <c r="E266" t="s">
+        <v>266</v>
+      </c>
+      <c r="F266" t="s">
+        <v>39</v>
+      </c>
+      <c r="G266" t="s">
+        <v>42</v>
+      </c>
+      <c r="H266" t="s">
+        <v>41</v>
+      </c>
+      <c r="I266" t="s">
+        <v>40</v>
+      </c>
+      <c r="J266">
+        <v>9</v>
+      </c>
+      <c r="K266" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="267" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A267" s="3">
+        <v>44179</v>
+      </c>
+      <c r="B267" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C267" s="4">
+        <v>2</v>
+      </c>
+      <c r="D267">
+        <v>21</v>
+      </c>
+      <c r="E267" t="s">
+        <v>266</v>
+      </c>
+      <c r="F267" t="s">
+        <v>87</v>
+      </c>
+      <c r="G267" t="s">
+        <v>108</v>
+      </c>
+      <c r="H267" t="s">
+        <v>89</v>
+      </c>
+      <c r="I267" t="s">
+        <v>90</v>
+      </c>
+      <c r="J267">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated code for multiple scripts within the NOAA project
</commit_message>
<xml_diff>
--- a/fishSurveys/data/fishSurveyData.xlsx
+++ b/fishSurveys/data/fishSurveyData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="9465" windowHeight="6615"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="9465" windowHeight="4920"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8510" uniqueCount="802">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8512" uniqueCount="803">
   <si>
     <t>date</t>
   </si>
@@ -2422,6 +2422,9 @@
   </si>
   <si>
     <t>Sparisoma rubripinne</t>
+  </si>
+  <si>
+    <t>`</t>
   </si>
 </sst>
 </file>
@@ -2772,11 +2775,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W1340"/>
+  <dimension ref="A1:W1341"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1332" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1341" sqref="B1341"/>
+      <pane ySplit="1" topLeftCell="A1335" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1341" sqref="E1341"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46990,6 +46993,20 @@
       </c>
       <c r="K1340" s="4" t="s">
         <v>178</v>
+      </c>
+    </row>
+    <row r="1341" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1341" s="3">
+        <v>44201</v>
+      </c>
+      <c r="B1341" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1341" s="4">
+        <v>1</v>
+      </c>
+      <c r="E1341" s="4" t="s">
+        <v>802</v>
       </c>
     </row>
   </sheetData>

</xml_diff>